<commit_message>
updated Test docs + BUG SUMMARY
Test documents have been updated to match the formats;

Test document for findTruckAndDiversion() now reflects the bugs encountered throughout function development
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/BB+WB_findTruckAndDiversion.xlsx
+++ b/Documents/Testing/TestsDocuments/BB+WB_findTruckAndDiversion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irish\Documents\SUM23-SFT221-NAA-4\Documents\Testing\TestsDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D69E4F-5EAF-4331-8314-1969F3F9ECEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1925CB-1D28-41E9-A1AF-9B0E1006E449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="174">
   <si>
     <t>Description</t>
   </si>
@@ -886,12 +886,39 @@
   <si>
     <t>BB_findTruckAndDiversion_2_6</t>
   </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>BUGS ENCOUNTERED?</t>
+  </si>
+  <si>
+    <t>YES;
+FUNCTION DIDN'T UPDATE THE orderOtherDay[] array but also didn't terminate the program.
+Faulty implementation of condition checks was corrected to pass this test.</t>
+  </si>
+  <si>
+    <t>NO;
+Corrected by debugging WB_findTruckAndDiversion_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES;
+FUNCTION DIDN'T CALCULATE THE MOST OPTIMISED ROUTE(as mentioned in the project document).
+Upon debugging the test case, it was discovered that the program got stuck in a corner and caused incorrect results.
+The function was modified to calculate diversion route starting from order destination to the point on truck route instead.
+(MAY NEED FURTHER IMPROVEMENT)
+</t>
+  </si>
+  <si>
+    <t>PLEASE NOTE: THE BUGS/ISSUES FOUND IN THIS FUNCTION WERE CORRECTED BY CHANGING THE IMPLEMENTATION TO PASS THE TEST CASES AS THE SCRIPT DIDN'T ALLOW PUSHING THE CODE TO THE REPOSITORY. Mentioned in worksheet titled "WHITEBOX" under "BUGS ENCOUNTERED?" column.
+Other minor issues have been documented in the code using comments.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -944,8 +971,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -980,6 +1028,16 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1198,10 +1256,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1239,6 +1299,53 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1257,6 +1364,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1266,82 +1382,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1620,10 +1712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4174010-3633-4931-93A9-0A7089B011F5}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:I10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1659,97 +1751,111 @@
       <c r="I3" s="27"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="28">
         <v>4</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="30"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="29"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="33"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="33"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="19"/>
     </row>
     <row r="9" spans="1:9" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="33"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:9" ht="228.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="21"/>
+    </row>
+    <row r="13" spans="1:9" ht="127.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="56" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A13:I13"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="A1:I1"/>
@@ -1767,7 +1873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AAE3EC-DDFB-4505-A7C8-4A197FCE6DA7}">
   <dimension ref="A1:G154"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A145" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G154"/>
     </sheetView>
   </sheetViews>
@@ -1782,10 +1888,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="16" t="s">
         <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1805,13 +1911,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="30" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1820,133 +1926,133 @@
       <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="36" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="46"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="46"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="46"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="46"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="37"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
       <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="46"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="4"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="46"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="37"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="46"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
       <c r="D10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="46"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="37"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
       <c r="D11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="46"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="37"/>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="5"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="47"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="38"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="39" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="8" t="s">
@@ -1955,195 +2061,195 @@
       <c r="E13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="G13" s="45" t="s">
+      <c r="G13" s="36" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="46"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="37"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="46"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="8"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="46"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="46"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="37"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
       <c r="D18" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="10"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="46"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="37"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="8"/>
       <c r="E19" s="10"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="46"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="37"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="8"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="46"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="37"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="8" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="10"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="46"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="37"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="10"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="46"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="37"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
       <c r="D23" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="10"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="46"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="37"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="10"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="46"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="37"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
       <c r="D25" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E25" s="10"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="46"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="37"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
       <c r="D26" s="8" t="s">
         <v>25</v>
       </c>
       <c r="E26" s="10"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="46"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="37"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
       <c r="D27" s="8"/>
       <c r="E27" s="10"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="46"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="37"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
       <c r="D28" s="8" t="s">
         <v>26</v>
       </c>
       <c r="E28" s="10"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="46"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="37"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
       <c r="D29" s="9"/>
       <c r="E29" s="11"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="47"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="38"/>
     </row>
     <row r="30" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="30" t="s">
         <v>29</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -2152,133 +2258,133 @@
       <c r="E30" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="G30" s="45" t="s">
+      <c r="G30" s="36" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
+      <c r="A31" s="31"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
       <c r="D31" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="46"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="37"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
       <c r="D32" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="46"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="37"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
       <c r="D33" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="46"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="37"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
       <c r="D34" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="46"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="37"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
       <c r="D35" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="6"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="46"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="37"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+      <c r="A36" s="31"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
       <c r="D36" s="4"/>
       <c r="E36" s="6"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="46"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="37"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
       <c r="D37" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E37" s="6"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="46"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="37"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
       <c r="D38" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E38" s="6"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="46"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="37"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
+      <c r="A39" s="31"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
       <c r="D39" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E39" s="6"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="46"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="37"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
+      <c r="A40" s="32"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
       <c r="D40" s="5"/>
       <c r="E40" s="7"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="47"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="38"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="39" t="s">
         <v>33</v>
       </c>
       <c r="D41" s="8" t="s">
@@ -2287,56 +2393,56 @@
       <c r="E41" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F41" s="19" t="s">
+      <c r="F41" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="G41" s="45" t="s">
+      <c r="G41" s="36" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
+      <c r="A42" s="40"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
       <c r="D42" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F42" s="20"/>
-      <c r="G42" s="46"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="37"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
       <c r="D43" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F43" s="20"/>
-      <c r="G43" s="46"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="37"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
       <c r="D44" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F44" s="20"/>
-      <c r="G44" s="46"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="37"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
       <c r="D45" s="8" t="s">
         <v>10</v>
       </c>
@@ -2344,187 +2450,187 @@
         <f xml:space="preserve"> 7</f>
         <v>7</v>
       </c>
-      <c r="F45" s="20"/>
-      <c r="G45" s="46"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="37"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
       <c r="D46" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F46" s="20"/>
-      <c r="G46" s="46"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="37"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
+      <c r="A47" s="40"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F47" s="20"/>
-      <c r="G47" s="46"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="37"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
+      <c r="A48" s="40"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
       <c r="D48" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E48" s="8"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="46"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="37"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
+      <c r="A49" s="40"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
       <c r="D49" s="8" t="s">
         <v>37</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F49" s="20"/>
-      <c r="G49" s="46"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="37"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
+      <c r="A50" s="40"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
       <c r="D50" s="8" t="s">
         <v>38</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F50" s="20"/>
-      <c r="G50" s="46"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="37"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="20"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
+      <c r="A51" s="40"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
       <c r="D51" s="8" t="s">
         <v>39</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F51" s="20"/>
-      <c r="G51" s="46"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="37"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="20"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
+      <c r="A52" s="40"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40"/>
       <c r="D52" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F52" s="20"/>
-      <c r="G52" s="46"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="37"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="20"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
+      <c r="A53" s="40"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="8" t="s">
         <v>41</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F53" s="20"/>
-      <c r="G53" s="46"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="37"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
+      <c r="A54" s="40"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
       <c r="D54" s="8"/>
       <c r="E54" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F54" s="20"/>
-      <c r="G54" s="46"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="37"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="20"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
+      <c r="A55" s="40"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
       <c r="D55" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F55" s="20"/>
-      <c r="G55" s="46"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="37"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="20"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="A56" s="40"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
       <c r="D56" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F56" s="20"/>
-      <c r="G56" s="46"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="37"/>
     </row>
     <row r="57" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="20"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
+      <c r="A57" s="40"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F57" s="20"/>
-      <c r="G57" s="46"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="37"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="20"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
+      <c r="A58" s="40"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
       <c r="D58" s="8" t="s">
         <v>44</v>
       </c>
       <c r="E58" s="8"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="46"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="37"/>
     </row>
     <row r="59" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="21"/>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
+      <c r="A59" s="41"/>
+      <c r="B59" s="41"/>
+      <c r="C59" s="41"/>
       <c r="D59" s="9"/>
       <c r="E59" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F59" s="21"/>
-      <c r="G59" s="47"/>
+      <c r="F59" s="41"/>
+      <c r="G59" s="38"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C60" s="30" t="s">
         <v>59</v>
       </c>
       <c r="D60" s="3" t="s">
@@ -2533,56 +2639,56 @@
       <c r="E60" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F60" s="16" t="s">
+      <c r="F60" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="G60" s="45" t="s">
+      <c r="G60" s="36" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="14"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
+      <c r="A61" s="31"/>
+      <c r="B61" s="31"/>
+      <c r="C61" s="31"/>
       <c r="D61" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F61" s="17"/>
-      <c r="G61" s="46"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="37"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="14"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
+      <c r="A62" s="31"/>
+      <c r="B62" s="31"/>
+      <c r="C62" s="31"/>
       <c r="D62" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F62" s="17"/>
-      <c r="G62" s="46"/>
+      <c r="F62" s="34"/>
+      <c r="G62" s="37"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
+      <c r="A63" s="31"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="31"/>
       <c r="D63" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F63" s="17"/>
-      <c r="G63" s="46"/>
+      <c r="F63" s="34"/>
+      <c r="G63" s="37"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="14"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
+      <c r="A64" s="31"/>
+      <c r="B64" s="31"/>
+      <c r="C64" s="31"/>
       <c r="D64" s="3" t="s">
         <v>10</v>
       </c>
@@ -2590,187 +2696,187 @@
         <f xml:space="preserve"> 7</f>
         <v>7</v>
       </c>
-      <c r="F64" s="17"/>
-      <c r="G64" s="46"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="37"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="14"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
+      <c r="A65" s="31"/>
+      <c r="B65" s="31"/>
+      <c r="C65" s="31"/>
       <c r="D65" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F65" s="17"/>
-      <c r="G65" s="46"/>
+      <c r="F65" s="34"/>
+      <c r="G65" s="37"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="14"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
+      <c r="A66" s="31"/>
+      <c r="B66" s="31"/>
+      <c r="C66" s="31"/>
       <c r="D66" s="4"/>
       <c r="E66" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F66" s="17"/>
-      <c r="G66" s="46"/>
+      <c r="F66" s="34"/>
+      <c r="G66" s="37"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="14"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
+      <c r="A67" s="31"/>
+      <c r="B67" s="31"/>
+      <c r="C67" s="31"/>
       <c r="D67" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E67" s="4"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="46"/>
+      <c r="F67" s="34"/>
+      <c r="G67" s="37"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="14"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
+      <c r="A68" s="31"/>
+      <c r="B68" s="31"/>
+      <c r="C68" s="31"/>
       <c r="D68" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F68" s="17"/>
-      <c r="G68" s="46"/>
+      <c r="F68" s="34"/>
+      <c r="G68" s="37"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="14"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="14"/>
+      <c r="A69" s="31"/>
+      <c r="B69" s="31"/>
+      <c r="C69" s="31"/>
       <c r="D69" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F69" s="17"/>
-      <c r="G69" s="46"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="37"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="14"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="14"/>
+      <c r="A70" s="31"/>
+      <c r="B70" s="31"/>
+      <c r="C70" s="31"/>
       <c r="D70" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F70" s="17"/>
-      <c r="G70" s="46"/>
+      <c r="F70" s="34"/>
+      <c r="G70" s="37"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="14"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
+      <c r="A71" s="31"/>
+      <c r="B71" s="31"/>
+      <c r="C71" s="31"/>
       <c r="D71" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F71" s="17"/>
-      <c r="G71" s="46"/>
+      <c r="F71" s="34"/>
+      <c r="G71" s="37"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="14"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
+      <c r="A72" s="31"/>
+      <c r="B72" s="31"/>
+      <c r="C72" s="31"/>
       <c r="D72" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F72" s="17"/>
-      <c r="G72" s="46"/>
+      <c r="F72" s="34"/>
+      <c r="G72" s="37"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="14"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
+      <c r="A73" s="31"/>
+      <c r="B73" s="31"/>
+      <c r="C73" s="31"/>
       <c r="D73" s="4"/>
       <c r="E73" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F73" s="17"/>
-      <c r="G73" s="46"/>
+      <c r="F73" s="34"/>
+      <c r="G73" s="37"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="14"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
+      <c r="A74" s="31"/>
+      <c r="B74" s="31"/>
+      <c r="C74" s="31"/>
       <c r="D74" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F74" s="17"/>
-      <c r="G74" s="46"/>
+      <c r="F74" s="34"/>
+      <c r="G74" s="37"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="14"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="14"/>
+      <c r="A75" s="31"/>
+      <c r="B75" s="31"/>
+      <c r="C75" s="31"/>
       <c r="D75" s="3" t="s">
         <v>63</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F75" s="17"/>
-      <c r="G75" s="46"/>
+      <c r="F75" s="34"/>
+      <c r="G75" s="37"/>
     </row>
     <row r="76" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A76" s="14"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="14"/>
+      <c r="A76" s="31"/>
+      <c r="B76" s="31"/>
+      <c r="C76" s="31"/>
       <c r="D76" s="4"/>
       <c r="E76" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F76" s="17"/>
-      <c r="G76" s="46"/>
+      <c r="F76" s="34"/>
+      <c r="G76" s="37"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="14"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
+      <c r="A77" s="31"/>
+      <c r="B77" s="31"/>
+      <c r="C77" s="31"/>
       <c r="D77" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E77" s="4"/>
-      <c r="F77" s="17"/>
-      <c r="G77" s="46"/>
+      <c r="F77" s="34"/>
+      <c r="G77" s="37"/>
     </row>
     <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="15"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="15"/>
+      <c r="A78" s="32"/>
+      <c r="B78" s="32"/>
+      <c r="C78" s="32"/>
       <c r="D78" s="7"/>
       <c r="E78" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F78" s="18"/>
-      <c r="G78" s="47"/>
+      <c r="F78" s="35"/>
+      <c r="G78" s="38"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="B79" s="19" t="s">
+      <c r="B79" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="C79" s="19" t="s">
+      <c r="C79" s="39" t="s">
         <v>73</v>
       </c>
       <c r="D79" s="8" t="s">
@@ -2779,56 +2885,56 @@
       <c r="E79" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F79" s="19" t="s">
+      <c r="F79" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="G79" s="45" t="s">
+      <c r="G79" s="36" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="20"/>
-      <c r="B80" s="20"/>
-      <c r="C80" s="20"/>
+      <c r="A80" s="40"/>
+      <c r="B80" s="40"/>
+      <c r="C80" s="40"/>
       <c r="D80" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F80" s="20"/>
-      <c r="G80" s="46"/>
+      <c r="F80" s="40"/>
+      <c r="G80" s="37"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="20"/>
-      <c r="B81" s="20"/>
-      <c r="C81" s="20"/>
+      <c r="A81" s="40"/>
+      <c r="B81" s="40"/>
+      <c r="C81" s="40"/>
       <c r="D81" s="8" t="s">
         <v>60</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F81" s="20"/>
-      <c r="G81" s="46"/>
+      <c r="F81" s="40"/>
+      <c r="G81" s="37"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="20"/>
-      <c r="B82" s="20"/>
-      <c r="C82" s="20"/>
+      <c r="A82" s="40"/>
+      <c r="B82" s="40"/>
+      <c r="C82" s="40"/>
       <c r="D82" s="8" t="s">
         <v>61</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F82" s="20"/>
-      <c r="G82" s="46"/>
+      <c r="F82" s="40"/>
+      <c r="G82" s="37"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="20"/>
-      <c r="B83" s="20"/>
-      <c r="C83" s="20"/>
+      <c r="A83" s="40"/>
+      <c r="B83" s="40"/>
+      <c r="C83" s="40"/>
       <c r="D83" s="8" t="s">
         <v>10</v>
       </c>
@@ -2836,176 +2942,176 @@
         <f xml:space="preserve"> 6</f>
         <v>6</v>
       </c>
-      <c r="F83" s="20"/>
-      <c r="G83" s="46"/>
+      <c r="F83" s="40"/>
+      <c r="G83" s="37"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A84" s="20"/>
-      <c r="B84" s="20"/>
-      <c r="C84" s="20"/>
+      <c r="A84" s="40"/>
+      <c r="B84" s="40"/>
+      <c r="C84" s="40"/>
       <c r="D84" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F84" s="20"/>
-      <c r="G84" s="46"/>
+      <c r="F84" s="40"/>
+      <c r="G84" s="37"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="20"/>
-      <c r="B85" s="20"/>
-      <c r="C85" s="20"/>
+      <c r="A85" s="40"/>
+      <c r="B85" s="40"/>
+      <c r="C85" s="40"/>
       <c r="D85" s="8"/>
       <c r="E85" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F85" s="20"/>
-      <c r="G85" s="46"/>
+      <c r="F85" s="40"/>
+      <c r="G85" s="37"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" s="20"/>
-      <c r="B86" s="20"/>
-      <c r="C86" s="20"/>
+      <c r="A86" s="40"/>
+      <c r="B86" s="40"/>
+      <c r="C86" s="40"/>
       <c r="D86" s="8" t="s">
         <v>74</v>
       </c>
       <c r="E86" s="8"/>
-      <c r="F86" s="20"/>
-      <c r="G86" s="46"/>
+      <c r="F86" s="40"/>
+      <c r="G86" s="37"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" s="20"/>
-      <c r="B87" s="20"/>
-      <c r="C87" s="20"/>
+      <c r="A87" s="40"/>
+      <c r="B87" s="40"/>
+      <c r="C87" s="40"/>
       <c r="D87" s="8" t="s">
         <v>75</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F87" s="20"/>
-      <c r="G87" s="46"/>
+      <c r="F87" s="40"/>
+      <c r="G87" s="37"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A88" s="20"/>
-      <c r="B88" s="20"/>
-      <c r="C88" s="20"/>
+      <c r="A88" s="40"/>
+      <c r="B88" s="40"/>
+      <c r="C88" s="40"/>
       <c r="D88" s="8" t="s">
         <v>76</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F88" s="20"/>
-      <c r="G88" s="46"/>
+      <c r="F88" s="40"/>
+      <c r="G88" s="37"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A89" s="20"/>
-      <c r="B89" s="20"/>
-      <c r="C89" s="20"/>
+      <c r="A89" s="40"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="40"/>
       <c r="D89" s="8" t="s">
         <v>77</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F89" s="20"/>
-      <c r="G89" s="46"/>
+      <c r="F89" s="40"/>
+      <c r="G89" s="37"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A90" s="20"/>
-      <c r="B90" s="20"/>
-      <c r="C90" s="20"/>
+      <c r="A90" s="40"/>
+      <c r="B90" s="40"/>
+      <c r="C90" s="40"/>
       <c r="D90" s="8" t="s">
         <v>78</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="F90" s="20"/>
-      <c r="G90" s="46"/>
+      <c r="F90" s="40"/>
+      <c r="G90" s="37"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A91" s="20"/>
-      <c r="B91" s="20"/>
-      <c r="C91" s="20"/>
+      <c r="A91" s="40"/>
+      <c r="B91" s="40"/>
+      <c r="C91" s="40"/>
       <c r="D91" s="8" t="s">
         <v>41</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="F91" s="20"/>
-      <c r="G91" s="46"/>
+      <c r="F91" s="40"/>
+      <c r="G91" s="37"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A92" s="20"/>
-      <c r="B92" s="20"/>
-      <c r="C92" s="20"/>
+      <c r="A92" s="40"/>
+      <c r="B92" s="40"/>
+      <c r="C92" s="40"/>
       <c r="D92" s="8"/>
       <c r="E92" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F92" s="20"/>
-      <c r="G92" s="46"/>
+      <c r="F92" s="40"/>
+      <c r="G92" s="37"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" s="20"/>
-      <c r="B93" s="20"/>
-      <c r="C93" s="20"/>
+      <c r="A93" s="40"/>
+      <c r="B93" s="40"/>
+      <c r="C93" s="40"/>
       <c r="D93" s="8" t="s">
         <v>79</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F93" s="20"/>
-      <c r="G93" s="46"/>
+      <c r="F93" s="40"/>
+      <c r="G93" s="37"/>
     </row>
     <row r="94" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A94" s="20"/>
-      <c r="B94" s="20"/>
-      <c r="C94" s="20"/>
+      <c r="A94" s="40"/>
+      <c r="B94" s="40"/>
+      <c r="C94" s="40"/>
       <c r="D94" s="8" t="s">
         <v>80</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F94" s="20"/>
-      <c r="G94" s="46"/>
+      <c r="F94" s="40"/>
+      <c r="G94" s="37"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A95" s="20"/>
-      <c r="B95" s="20"/>
-      <c r="C95" s="20"/>
+      <c r="A95" s="40"/>
+      <c r="B95" s="40"/>
+      <c r="C95" s="40"/>
       <c r="D95" s="8"/>
       <c r="E95" s="8"/>
-      <c r="F95" s="20"/>
-      <c r="G95" s="46"/>
+      <c r="F95" s="40"/>
+      <c r="G95" s="37"/>
     </row>
     <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="21"/>
-      <c r="B96" s="21"/>
-      <c r="C96" s="21"/>
+      <c r="A96" s="41"/>
+      <c r="B96" s="41"/>
+      <c r="C96" s="41"/>
       <c r="D96" s="9" t="s">
         <v>44</v>
       </c>
       <c r="E96" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F96" s="21"/>
-      <c r="G96" s="47"/>
+      <c r="F96" s="41"/>
+      <c r="G96" s="38"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A97" s="13" t="s">
+      <c r="A97" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="B97" s="13" t="s">
+      <c r="B97" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="C97" s="13" t="s">
+      <c r="C97" s="30" t="s">
         <v>89</v>
       </c>
       <c r="D97" s="3" t="s">
@@ -3014,56 +3120,56 @@
       <c r="E97" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F97" s="16" t="s">
+      <c r="F97" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="G97" s="45" t="s">
+      <c r="G97" s="36" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A98" s="14"/>
-      <c r="B98" s="14"/>
-      <c r="C98" s="14"/>
+      <c r="A98" s="31"/>
+      <c r="B98" s="31"/>
+      <c r="C98" s="31"/>
       <c r="D98" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F98" s="17"/>
-      <c r="G98" s="46"/>
+      <c r="F98" s="34"/>
+      <c r="G98" s="37"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A99" s="14"/>
-      <c r="B99" s="14"/>
-      <c r="C99" s="14"/>
+      <c r="A99" s="31"/>
+      <c r="B99" s="31"/>
+      <c r="C99" s="31"/>
       <c r="D99" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F99" s="17"/>
-      <c r="G99" s="46"/>
+      <c r="F99" s="34"/>
+      <c r="G99" s="37"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A100" s="14"/>
-      <c r="B100" s="14"/>
-      <c r="C100" s="14"/>
+      <c r="A100" s="31"/>
+      <c r="B100" s="31"/>
+      <c r="C100" s="31"/>
       <c r="D100" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F100" s="17"/>
-      <c r="G100" s="46"/>
+      <c r="F100" s="34"/>
+      <c r="G100" s="37"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A101" s="14"/>
-      <c r="B101" s="14"/>
-      <c r="C101" s="14"/>
+      <c r="A101" s="31"/>
+      <c r="B101" s="31"/>
+      <c r="C101" s="31"/>
       <c r="D101" s="3" t="s">
         <v>11</v>
       </c>
@@ -3071,174 +3177,174 @@
         <f xml:space="preserve"> 6</f>
         <v>6</v>
       </c>
-      <c r="F101" s="17"/>
-      <c r="G101" s="46"/>
+      <c r="F101" s="34"/>
+      <c r="G101" s="37"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A102" s="14"/>
-      <c r="B102" s="14"/>
-      <c r="C102" s="14"/>
+      <c r="A102" s="31"/>
+      <c r="B102" s="31"/>
+      <c r="C102" s="31"/>
       <c r="D102" s="4"/>
       <c r="E102" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F102" s="17"/>
-      <c r="G102" s="46"/>
+      <c r="F102" s="34"/>
+      <c r="G102" s="37"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A103" s="14"/>
-      <c r="B103" s="14"/>
-      <c r="C103" s="14"/>
+      <c r="A103" s="31"/>
+      <c r="B103" s="31"/>
+      <c r="C103" s="31"/>
       <c r="D103" s="3" t="s">
         <v>74</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F103" s="17"/>
-      <c r="G103" s="46"/>
+      <c r="F103" s="34"/>
+      <c r="G103" s="37"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A104" s="14"/>
-      <c r="B104" s="14"/>
-      <c r="C104" s="14"/>
+      <c r="A104" s="31"/>
+      <c r="B104" s="31"/>
+      <c r="C104" s="31"/>
       <c r="D104" s="3" t="s">
         <v>75</v>
       </c>
       <c r="E104" s="4"/>
-      <c r="F104" s="17"/>
-      <c r="G104" s="46"/>
+      <c r="F104" s="34"/>
+      <c r="G104" s="37"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A105" s="14"/>
-      <c r="B105" s="14"/>
-      <c r="C105" s="14"/>
+      <c r="A105" s="31"/>
+      <c r="B105" s="31"/>
+      <c r="C105" s="31"/>
       <c r="D105" s="3" t="s">
         <v>76</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F105" s="17"/>
-      <c r="G105" s="46"/>
+      <c r="F105" s="34"/>
+      <c r="G105" s="37"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A106" s="14"/>
-      <c r="B106" s="14"/>
-      <c r="C106" s="14"/>
+      <c r="A106" s="31"/>
+      <c r="B106" s="31"/>
+      <c r="C106" s="31"/>
       <c r="D106" s="3" t="s">
         <v>77</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F106" s="17"/>
-      <c r="G106" s="46"/>
+      <c r="F106" s="34"/>
+      <c r="G106" s="37"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A107" s="14"/>
-      <c r="B107" s="14"/>
-      <c r="C107" s="14"/>
+      <c r="A107" s="31"/>
+      <c r="B107" s="31"/>
+      <c r="C107" s="31"/>
       <c r="D107" s="3" t="s">
         <v>78</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F107" s="17"/>
-      <c r="G107" s="46"/>
+      <c r="F107" s="34"/>
+      <c r="G107" s="37"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A108" s="14"/>
-      <c r="B108" s="14"/>
-      <c r="C108" s="14"/>
+      <c r="A108" s="31"/>
+      <c r="B108" s="31"/>
+      <c r="C108" s="31"/>
       <c r="D108" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F108" s="17"/>
-      <c r="G108" s="46"/>
+      <c r="F108" s="34"/>
+      <c r="G108" s="37"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A109" s="14"/>
-      <c r="B109" s="14"/>
-      <c r="C109" s="14"/>
+      <c r="A109" s="31"/>
+      <c r="B109" s="31"/>
+      <c r="C109" s="31"/>
       <c r="D109" s="4"/>
       <c r="E109" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F109" s="17"/>
-      <c r="G109" s="46"/>
+      <c r="F109" s="34"/>
+      <c r="G109" s="37"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A110" s="14"/>
-      <c r="B110" s="14"/>
-      <c r="C110" s="14"/>
+      <c r="A110" s="31"/>
+      <c r="B110" s="31"/>
+      <c r="C110" s="31"/>
       <c r="D110" s="3" t="s">
         <v>92</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F110" s="17"/>
-      <c r="G110" s="46"/>
+      <c r="F110" s="34"/>
+      <c r="G110" s="37"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A111" s="14"/>
-      <c r="B111" s="14"/>
-      <c r="C111" s="14"/>
+      <c r="A111" s="31"/>
+      <c r="B111" s="31"/>
+      <c r="C111" s="31"/>
       <c r="D111" s="3" t="s">
         <v>80</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F111" s="17"/>
-      <c r="G111" s="46"/>
+      <c r="F111" s="34"/>
+      <c r="G111" s="37"/>
     </row>
     <row r="112" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A112" s="14"/>
-      <c r="B112" s="14"/>
-      <c r="C112" s="14"/>
+      <c r="A112" s="31"/>
+      <c r="B112" s="31"/>
+      <c r="C112" s="31"/>
       <c r="D112" s="4"/>
       <c r="E112" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F112" s="17"/>
-      <c r="G112" s="46"/>
+      <c r="F112" s="34"/>
+      <c r="G112" s="37"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A113" s="14"/>
-      <c r="B113" s="14"/>
-      <c r="C113" s="14"/>
+      <c r="A113" s="31"/>
+      <c r="B113" s="31"/>
+      <c r="C113" s="31"/>
       <c r="D113" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E113" s="4"/>
-      <c r="F113" s="17"/>
-      <c r="G113" s="46"/>
+      <c r="F113" s="34"/>
+      <c r="G113" s="37"/>
     </row>
     <row r="114" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="15"/>
-      <c r="B114" s="15"/>
-      <c r="C114" s="15"/>
+      <c r="A114" s="32"/>
+      <c r="B114" s="32"/>
+      <c r="C114" s="32"/>
       <c r="D114" s="5"/>
       <c r="E114" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F114" s="18"/>
-      <c r="G114" s="47"/>
+      <c r="F114" s="35"/>
+      <c r="G114" s="38"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A115" s="19" t="s">
+      <c r="A115" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="B115" s="19" t="s">
+      <c r="B115" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="C115" s="19" t="s">
+      <c r="C115" s="39" t="s">
         <v>99</v>
       </c>
       <c r="D115" s="8" t="s">
@@ -3247,56 +3353,56 @@
       <c r="E115" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F115" s="19" t="s">
+      <c r="F115" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="G115" s="45" t="s">
+      <c r="G115" s="36" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A116" s="20"/>
-      <c r="B116" s="20"/>
-      <c r="C116" s="20"/>
+      <c r="A116" s="40"/>
+      <c r="B116" s="40"/>
+      <c r="C116" s="40"/>
       <c r="D116" s="8" t="s">
         <v>100</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="F116" s="20"/>
-      <c r="G116" s="46"/>
+      <c r="F116" s="40"/>
+      <c r="G116" s="37"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A117" s="20"/>
-      <c r="B117" s="20"/>
-      <c r="C117" s="20"/>
+      <c r="A117" s="40"/>
+      <c r="B117" s="40"/>
+      <c r="C117" s="40"/>
       <c r="D117" s="8" t="s">
         <v>60</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="F117" s="20"/>
-      <c r="G117" s="46"/>
+      <c r="F117" s="40"/>
+      <c r="G117" s="37"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A118" s="20"/>
-      <c r="B118" s="20"/>
-      <c r="C118" s="20"/>
+      <c r="A118" s="40"/>
+      <c r="B118" s="40"/>
+      <c r="C118" s="40"/>
       <c r="D118" s="8" t="s">
         <v>61</v>
       </c>
       <c r="E118" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F118" s="20"/>
-      <c r="G118" s="46"/>
+      <c r="F118" s="40"/>
+      <c r="G118" s="37"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A119" s="20"/>
-      <c r="B119" s="20"/>
-      <c r="C119" s="20"/>
+      <c r="A119" s="40"/>
+      <c r="B119" s="40"/>
+      <c r="C119" s="40"/>
       <c r="D119" s="8" t="s">
         <v>10</v>
       </c>
@@ -3304,181 +3410,181 @@
         <f xml:space="preserve"> 4</f>
         <v>4</v>
       </c>
-      <c r="F119" s="20"/>
-      <c r="G119" s="46"/>
+      <c r="F119" s="40"/>
+      <c r="G119" s="37"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A120" s="20"/>
-      <c r="B120" s="20"/>
-      <c r="C120" s="20"/>
+      <c r="A120" s="40"/>
+      <c r="B120" s="40"/>
+      <c r="C120" s="40"/>
       <c r="D120" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F120" s="20"/>
-      <c r="G120" s="46"/>
+      <c r="F120" s="40"/>
+      <c r="G120" s="37"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A121" s="20"/>
-      <c r="B121" s="20"/>
-      <c r="C121" s="20"/>
+      <c r="A121" s="40"/>
+      <c r="B121" s="40"/>
+      <c r="C121" s="40"/>
       <c r="D121" s="8"/>
       <c r="E121" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F121" s="20"/>
-      <c r="G121" s="46"/>
+      <c r="F121" s="40"/>
+      <c r="G121" s="37"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A122" s="20"/>
-      <c r="B122" s="20"/>
-      <c r="C122" s="20"/>
+      <c r="A122" s="40"/>
+      <c r="B122" s="40"/>
+      <c r="C122" s="40"/>
       <c r="D122" s="8" t="s">
         <v>101</v>
       </c>
       <c r="E122" s="8"/>
-      <c r="F122" s="20"/>
-      <c r="G122" s="46"/>
+      <c r="F122" s="40"/>
+      <c r="G122" s="37"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A123" s="20"/>
-      <c r="B123" s="20"/>
-      <c r="C123" s="20"/>
+      <c r="A123" s="40"/>
+      <c r="B123" s="40"/>
+      <c r="C123" s="40"/>
       <c r="D123" s="8" t="s">
         <v>37</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F123" s="20"/>
-      <c r="G123" s="46"/>
+      <c r="F123" s="40"/>
+      <c r="G123" s="37"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A124" s="20"/>
-      <c r="B124" s="20"/>
-      <c r="C124" s="20"/>
+      <c r="A124" s="40"/>
+      <c r="B124" s="40"/>
+      <c r="C124" s="40"/>
       <c r="D124" s="8" t="s">
         <v>102</v>
       </c>
       <c r="E124" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F124" s="20"/>
-      <c r="G124" s="46"/>
+      <c r="F124" s="40"/>
+      <c r="G124" s="37"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A125" s="20"/>
-      <c r="B125" s="20"/>
-      <c r="C125" s="20"/>
+      <c r="A125" s="40"/>
+      <c r="B125" s="40"/>
+      <c r="C125" s="40"/>
       <c r="D125" s="8" t="s">
         <v>103</v>
       </c>
       <c r="E125" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F125" s="20"/>
-      <c r="G125" s="46"/>
+      <c r="F125" s="40"/>
+      <c r="G125" s="37"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A126" s="20"/>
-      <c r="B126" s="20"/>
-      <c r="C126" s="20"/>
+      <c r="A126" s="40"/>
+      <c r="B126" s="40"/>
+      <c r="C126" s="40"/>
       <c r="D126" s="8" t="s">
         <v>104</v>
       </c>
       <c r="E126" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F126" s="20"/>
-      <c r="G126" s="46"/>
+      <c r="F126" s="40"/>
+      <c r="G126" s="37"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A127" s="20"/>
-      <c r="B127" s="20"/>
-      <c r="C127" s="20"/>
+      <c r="A127" s="40"/>
+      <c r="B127" s="40"/>
+      <c r="C127" s="40"/>
       <c r="D127" s="8" t="s">
         <v>105</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="F127" s="20"/>
-      <c r="G127" s="46"/>
+      <c r="F127" s="40"/>
+      <c r="G127" s="37"/>
     </row>
     <row r="128" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A128" s="20"/>
-      <c r="B128" s="20"/>
-      <c r="C128" s="20"/>
+      <c r="A128" s="40"/>
+      <c r="B128" s="40"/>
+      <c r="C128" s="40"/>
       <c r="D128" s="8"/>
       <c r="E128" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="F128" s="20"/>
-      <c r="G128" s="46"/>
+      <c r="F128" s="40"/>
+      <c r="G128" s="37"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A129" s="20"/>
-      <c r="B129" s="20"/>
-      <c r="C129" s="20"/>
+      <c r="A129" s="40"/>
+      <c r="B129" s="40"/>
+      <c r="C129" s="40"/>
       <c r="D129" s="8" t="s">
         <v>79</v>
       </c>
       <c r="E129" s="8"/>
-      <c r="F129" s="20"/>
-      <c r="G129" s="46"/>
+      <c r="F129" s="40"/>
+      <c r="G129" s="37"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A130" s="20"/>
-      <c r="B130" s="20"/>
-      <c r="C130" s="20"/>
+      <c r="A130" s="40"/>
+      <c r="B130" s="40"/>
+      <c r="C130" s="40"/>
       <c r="D130" s="8" t="s">
         <v>106</v>
       </c>
       <c r="E130" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F130" s="20"/>
-      <c r="G130" s="46"/>
+      <c r="F130" s="40"/>
+      <c r="G130" s="37"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A131" s="20"/>
-      <c r="B131" s="20"/>
-      <c r="C131" s="20"/>
+      <c r="A131" s="40"/>
+      <c r="B131" s="40"/>
+      <c r="C131" s="40"/>
       <c r="D131" s="8"/>
       <c r="E131" s="10"/>
-      <c r="F131" s="20"/>
-      <c r="G131" s="46"/>
+      <c r="F131" s="40"/>
+      <c r="G131" s="37"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A132" s="20"/>
-      <c r="B132" s="20"/>
-      <c r="C132" s="20"/>
+      <c r="A132" s="40"/>
+      <c r="B132" s="40"/>
+      <c r="C132" s="40"/>
       <c r="D132" s="8" t="s">
         <v>44</v>
       </c>
       <c r="E132" s="10"/>
-      <c r="F132" s="20"/>
-      <c r="G132" s="46"/>
+      <c r="F132" s="40"/>
+      <c r="G132" s="37"/>
     </row>
     <row r="133" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="21"/>
-      <c r="B133" s="21"/>
-      <c r="C133" s="21"/>
+      <c r="A133" s="41"/>
+      <c r="B133" s="41"/>
+      <c r="C133" s="41"/>
       <c r="D133" s="9"/>
       <c r="E133" s="11"/>
-      <c r="F133" s="21"/>
-      <c r="G133" s="47"/>
+      <c r="F133" s="41"/>
+      <c r="G133" s="38"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A134" s="13" t="s">
+      <c r="A134" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="B134" s="13" t="s">
+      <c r="B134" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="C134" s="13" t="s">
+      <c r="C134" s="30" t="s">
         <v>113</v>
       </c>
       <c r="D134" s="3" t="s">
@@ -3487,301 +3593,301 @@
       <c r="E134" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F134" s="16" t="s">
+      <c r="F134" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="G134" s="45" t="s">
+      <c r="G134" s="36" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A135" s="14"/>
-      <c r="B135" s="14"/>
-      <c r="C135" s="14"/>
+      <c r="A135" s="31"/>
+      <c r="B135" s="31"/>
+      <c r="C135" s="31"/>
       <c r="D135" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F135" s="17"/>
-      <c r="G135" s="46"/>
+      <c r="F135" s="34"/>
+      <c r="G135" s="37"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A136" s="14"/>
-      <c r="B136" s="14"/>
-      <c r="C136" s="14"/>
+      <c r="A136" s="31"/>
+      <c r="B136" s="31"/>
+      <c r="C136" s="31"/>
       <c r="D136" s="3" t="s">
         <v>114</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F136" s="17"/>
-      <c r="G136" s="46"/>
+      <c r="F136" s="34"/>
+      <c r="G136" s="37"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A137" s="14"/>
-      <c r="B137" s="14"/>
-      <c r="C137" s="14"/>
+      <c r="A137" s="31"/>
+      <c r="B137" s="31"/>
+      <c r="C137" s="31"/>
       <c r="D137" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E137" s="4"/>
-      <c r="F137" s="17"/>
-      <c r="G137" s="46"/>
+      <c r="F137" s="34"/>
+      <c r="G137" s="37"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A138" s="14"/>
-      <c r="B138" s="14"/>
-      <c r="C138" s="14"/>
+      <c r="A138" s="31"/>
+      <c r="B138" s="31"/>
+      <c r="C138" s="31"/>
       <c r="D138" s="3" t="s">
         <v>115</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F138" s="17"/>
-      <c r="G138" s="46"/>
+      <c r="F138" s="34"/>
+      <c r="G138" s="37"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A139" s="14"/>
-      <c r="B139" s="14"/>
-      <c r="C139" s="14"/>
+      <c r="A139" s="31"/>
+      <c r="B139" s="31"/>
+      <c r="C139" s="31"/>
       <c r="D139" s="3" t="s">
         <v>116</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F139" s="17"/>
-      <c r="G139" s="46"/>
+      <c r="F139" s="34"/>
+      <c r="G139" s="37"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A140" s="14"/>
-      <c r="B140" s="14"/>
-      <c r="C140" s="14"/>
+      <c r="A140" s="31"/>
+      <c r="B140" s="31"/>
+      <c r="C140" s="31"/>
       <c r="D140" s="4"/>
       <c r="E140" s="3">
         <f xml:space="preserve"> 4</f>
         <v>4</v>
       </c>
-      <c r="F140" s="17"/>
-      <c r="G140" s="46"/>
+      <c r="F140" s="34"/>
+      <c r="G140" s="37"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A141" s="14"/>
-      <c r="B141" s="14"/>
-      <c r="C141" s="14"/>
+      <c r="A141" s="31"/>
+      <c r="B141" s="31"/>
+      <c r="C141" s="31"/>
       <c r="D141" s="3" t="s">
         <v>101</v>
       </c>
       <c r="E141" s="4"/>
-      <c r="F141" s="17"/>
-      <c r="G141" s="46"/>
+      <c r="F141" s="34"/>
+      <c r="G141" s="37"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A142" s="14"/>
-      <c r="B142" s="14"/>
-      <c r="C142" s="14"/>
+      <c r="A142" s="31"/>
+      <c r="B142" s="31"/>
+      <c r="C142" s="31"/>
       <c r="D142" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F142" s="17"/>
-      <c r="G142" s="46"/>
+      <c r="F142" s="34"/>
+      <c r="G142" s="37"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A143" s="14"/>
-      <c r="B143" s="14"/>
-      <c r="C143" s="14"/>
+      <c r="A143" s="31"/>
+      <c r="B143" s="31"/>
+      <c r="C143" s="31"/>
       <c r="D143" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F143" s="17"/>
-      <c r="G143" s="46"/>
+      <c r="F143" s="34"/>
+      <c r="G143" s="37"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A144" s="14"/>
-      <c r="B144" s="14"/>
-      <c r="C144" s="14"/>
+      <c r="A144" s="31"/>
+      <c r="B144" s="31"/>
+      <c r="C144" s="31"/>
       <c r="D144" s="3" t="s">
         <v>103</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F144" s="17"/>
-      <c r="G144" s="46"/>
+      <c r="F144" s="34"/>
+      <c r="G144" s="37"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A145" s="14"/>
-      <c r="B145" s="14"/>
-      <c r="C145" s="14"/>
+      <c r="A145" s="31"/>
+      <c r="B145" s="31"/>
+      <c r="C145" s="31"/>
       <c r="D145" s="3" t="s">
         <v>104</v>
       </c>
       <c r="E145" s="4"/>
-      <c r="F145" s="17"/>
-      <c r="G145" s="46"/>
+      <c r="F145" s="34"/>
+      <c r="G145" s="37"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A146" s="14"/>
-      <c r="B146" s="14"/>
-      <c r="C146" s="14"/>
+      <c r="A146" s="31"/>
+      <c r="B146" s="31"/>
+      <c r="C146" s="31"/>
       <c r="D146" s="3" t="s">
         <v>105</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F146" s="17"/>
-      <c r="G146" s="46"/>
+      <c r="F146" s="34"/>
+      <c r="G146" s="37"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A147" s="14"/>
-      <c r="B147" s="14"/>
-      <c r="C147" s="14"/>
+      <c r="A147" s="31"/>
+      <c r="B147" s="31"/>
+      <c r="C147" s="31"/>
       <c r="D147" s="4"/>
       <c r="E147" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F147" s="17"/>
-      <c r="G147" s="46"/>
+      <c r="F147" s="34"/>
+      <c r="G147" s="37"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A148" s="14"/>
-      <c r="B148" s="14"/>
-      <c r="C148" s="14"/>
+      <c r="A148" s="31"/>
+      <c r="B148" s="31"/>
+      <c r="C148" s="31"/>
       <c r="D148" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F148" s="17"/>
-      <c r="G148" s="46"/>
+      <c r="F148" s="34"/>
+      <c r="G148" s="37"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A149" s="14"/>
-      <c r="B149" s="14"/>
-      <c r="C149" s="14"/>
+      <c r="A149" s="31"/>
+      <c r="B149" s="31"/>
+      <c r="C149" s="31"/>
       <c r="D149" s="3" t="s">
         <v>106</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F149" s="17"/>
-      <c r="G149" s="46"/>
+      <c r="F149" s="34"/>
+      <c r="G149" s="37"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A150" s="14"/>
-      <c r="B150" s="14"/>
-      <c r="C150" s="14"/>
+      <c r="A150" s="31"/>
+      <c r="B150" s="31"/>
+      <c r="C150" s="31"/>
       <c r="D150" s="4"/>
       <c r="E150" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F150" s="17"/>
-      <c r="G150" s="46"/>
+      <c r="F150" s="34"/>
+      <c r="G150" s="37"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A151" s="14"/>
-      <c r="B151" s="14"/>
-      <c r="C151" s="14"/>
+      <c r="A151" s="31"/>
+      <c r="B151" s="31"/>
+      <c r="C151" s="31"/>
       <c r="D151" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F151" s="17"/>
-      <c r="G151" s="46"/>
+      <c r="F151" s="34"/>
+      <c r="G151" s="37"/>
     </row>
     <row r="152" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A152" s="14"/>
-      <c r="B152" s="14"/>
-      <c r="C152" s="14"/>
+      <c r="A152" s="31"/>
+      <c r="B152" s="31"/>
+      <c r="C152" s="31"/>
       <c r="D152" s="6"/>
       <c r="E152" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F152" s="17"/>
-      <c r="G152" s="46"/>
+      <c r="F152" s="34"/>
+      <c r="G152" s="37"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A153" s="14"/>
-      <c r="B153" s="14"/>
-      <c r="C153" s="14"/>
+      <c r="A153" s="31"/>
+      <c r="B153" s="31"/>
+      <c r="C153" s="31"/>
       <c r="D153" s="6"/>
       <c r="E153" s="4"/>
-      <c r="F153" s="17"/>
-      <c r="G153" s="46"/>
+      <c r="F153" s="34"/>
+      <c r="G153" s="37"/>
     </row>
     <row r="154" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="15"/>
-      <c r="B154" s="15"/>
-      <c r="C154" s="15"/>
+      <c r="A154" s="32"/>
+      <c r="B154" s="32"/>
+      <c r="C154" s="32"/>
       <c r="D154" s="7"/>
       <c r="E154" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F154" s="18"/>
-      <c r="G154" s="47"/>
+      <c r="F154" s="35"/>
+      <c r="G154" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="A13:A29"/>
+    <mergeCell ref="B13:B29"/>
+    <mergeCell ref="C13:C29"/>
+    <mergeCell ref="F13:F29"/>
+    <mergeCell ref="G13:G29"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="C2:C12"/>
+    <mergeCell ref="F2:F12"/>
+    <mergeCell ref="G2:G12"/>
+    <mergeCell ref="A41:A59"/>
+    <mergeCell ref="B41:B59"/>
+    <mergeCell ref="C41:C59"/>
+    <mergeCell ref="F41:F59"/>
+    <mergeCell ref="G41:G59"/>
+    <mergeCell ref="A30:A40"/>
+    <mergeCell ref="B30:B40"/>
+    <mergeCell ref="C30:C40"/>
+    <mergeCell ref="F30:F40"/>
+    <mergeCell ref="G30:G40"/>
+    <mergeCell ref="A79:A96"/>
+    <mergeCell ref="B79:B96"/>
+    <mergeCell ref="C79:C96"/>
+    <mergeCell ref="F79:F96"/>
+    <mergeCell ref="G79:G96"/>
+    <mergeCell ref="A60:A78"/>
+    <mergeCell ref="B60:B78"/>
+    <mergeCell ref="C60:C78"/>
+    <mergeCell ref="F60:F78"/>
+    <mergeCell ref="G60:G78"/>
+    <mergeCell ref="A115:A133"/>
+    <mergeCell ref="B115:B133"/>
+    <mergeCell ref="C115:C133"/>
+    <mergeCell ref="F115:F133"/>
+    <mergeCell ref="G115:G133"/>
+    <mergeCell ref="A97:A114"/>
+    <mergeCell ref="B97:B114"/>
+    <mergeCell ref="C97:C114"/>
+    <mergeCell ref="F97:F114"/>
+    <mergeCell ref="G97:G114"/>
     <mergeCell ref="A134:A154"/>
     <mergeCell ref="B134:B154"/>
     <mergeCell ref="C134:C154"/>
     <mergeCell ref="F134:F154"/>
     <mergeCell ref="G134:G154"/>
-    <mergeCell ref="A97:A114"/>
-    <mergeCell ref="B97:B114"/>
-    <mergeCell ref="C97:C114"/>
-    <mergeCell ref="F97:F114"/>
-    <mergeCell ref="G97:G114"/>
-    <mergeCell ref="A115:A133"/>
-    <mergeCell ref="B115:B133"/>
-    <mergeCell ref="C115:C133"/>
-    <mergeCell ref="F115:F133"/>
-    <mergeCell ref="G115:G133"/>
-    <mergeCell ref="A60:A78"/>
-    <mergeCell ref="B60:B78"/>
-    <mergeCell ref="C60:C78"/>
-    <mergeCell ref="F60:F78"/>
-    <mergeCell ref="G60:G78"/>
-    <mergeCell ref="A79:A96"/>
-    <mergeCell ref="B79:B96"/>
-    <mergeCell ref="C79:C96"/>
-    <mergeCell ref="F79:F96"/>
-    <mergeCell ref="G79:G96"/>
-    <mergeCell ref="A30:A40"/>
-    <mergeCell ref="B30:B40"/>
-    <mergeCell ref="C30:C40"/>
-    <mergeCell ref="F30:F40"/>
-    <mergeCell ref="G30:G40"/>
-    <mergeCell ref="A41:A59"/>
-    <mergeCell ref="B41:B59"/>
-    <mergeCell ref="C41:C59"/>
-    <mergeCell ref="F41:F59"/>
-    <mergeCell ref="G41:G59"/>
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="C2:C12"/>
-    <mergeCell ref="F2:F12"/>
-    <mergeCell ref="G2:G12"/>
-    <mergeCell ref="A13:A29"/>
-    <mergeCell ref="B13:B29"/>
-    <mergeCell ref="C13:C29"/>
-    <mergeCell ref="F13:F29"/>
-    <mergeCell ref="G13:G29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3790,10 +3896,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G78"/>
+      <selection activeCell="H30" sqref="H30:H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3803,14 +3909,16 @@
     <col min="3" max="3" width="28.44140625" customWidth="1"/>
     <col min="4" max="4" width="59.21875" customWidth="1"/>
     <col min="5" max="5" width="77" customWidth="1"/>
-    <col min="6" max="7" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
+    <col min="8" max="8" width="29.5546875" style="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="16" t="s">
         <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -3828,128 +3936,144 @@
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="H1" s="48" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="30" t="s">
         <v>147</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="36" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="40" t="s">
+      <c r="H2" s="53" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="46"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="46"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="46"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="46"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="46"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="46"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="46"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="46"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="46"/>
-    </row>
-    <row r="12" spans="1:7" ht="130.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="47"/>
-    </row>
-    <row r="13" spans="1:7" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="E3" s="45"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="54"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="54"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="54"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="54"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="54"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="54"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="54"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="54"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="54"/>
+    </row>
+    <row r="12" spans="1:8" ht="130.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="55"/>
+    </row>
+    <row r="13" spans="1:8" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="39" t="s">
         <v>149</v>
       </c>
       <c r="D13" s="42" t="s">
@@ -3958,278 +4082,310 @@
       <c r="E13" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="G13" s="45" t="s">
+      <c r="G13" s="36" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
+      <c r="H13" s="49" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="43"/>
       <c r="E14" s="43"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="46"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="50"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="43"/>
       <c r="E15" s="43"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="46"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="50"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="46"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="50"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="43"/>
       <c r="E17" s="43"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="46"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="50"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
       <c r="D18" s="43"/>
       <c r="E18" s="43"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="46"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="50"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="43"/>
       <c r="E19" s="43"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="46"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="50"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="43"/>
       <c r="E20" s="43"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="46"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="50"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="40"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="43"/>
       <c r="E21" s="43"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="46"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="50"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="43"/>
       <c r="E22" s="43"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="46"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="50"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="40"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
       <c r="D23" s="43"/>
       <c r="E23" s="43"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="46"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="50"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="43"/>
       <c r="E24" s="43"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="46"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="50"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
       <c r="D25" s="43"/>
       <c r="E25" s="43"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="46"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="50"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="40"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
       <c r="D26" s="43"/>
       <c r="E26" s="43"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="46"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="50"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="40"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
       <c r="D27" s="43"/>
       <c r="E27" s="43"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="46"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="50"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
       <c r="D28" s="43"/>
       <c r="E28" s="43"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="46"/>
-    </row>
-    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="50"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
       <c r="D29" s="44"/>
       <c r="E29" s="44"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="47"/>
-    </row>
-    <row r="30" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
+      <c r="F29" s="41"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="51"/>
+    </row>
+    <row r="30" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="D30" s="39" t="s">
+      <c r="D30" s="47" t="s">
         <v>151</v>
       </c>
-      <c r="E30" s="39" t="s">
+      <c r="E30" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="G30" s="45" t="s">
+      <c r="G30" s="36" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="46"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="46"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="46"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="46"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="46"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="46"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="46"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="46"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="46"/>
-    </row>
-    <row r="40" spans="1:7" ht="277.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="47"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="19" t="s">
+      <c r="H30" s="49" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="31"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="50"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="31"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="50"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="50"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="31"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="50"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="31"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="50"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="31"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="50"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="31"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="50"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="31"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="50"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="31"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="50"/>
+    </row>
+    <row r="40" spans="1:8" ht="277.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="32"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="51"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D41" s="42" t="s">
@@ -4238,372 +4394,424 @@
       <c r="E41" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="F41" s="19" t="s">
+      <c r="F41" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="G41" s="45" t="s">
+      <c r="G41" s="36" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
+      <c r="H41" s="53" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="40"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
       <c r="D42" s="43"/>
       <c r="E42" s="43"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="46"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="54"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
       <c r="D43" s="43"/>
       <c r="E43" s="43"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="46"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="54"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
       <c r="D44" s="43"/>
       <c r="E44" s="43"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="46"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="54"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
       <c r="D45" s="43"/>
       <c r="E45" s="43"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="46"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="54"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
       <c r="D46" s="43"/>
       <c r="E46" s="43"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="46"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="54"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="40"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
       <c r="D47" s="43"/>
       <c r="E47" s="43"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="46"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="54"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="40"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
       <c r="D48" s="43"/>
       <c r="E48" s="43"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="46"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="54"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="40"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
       <c r="D49" s="43"/>
       <c r="E49" s="43"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="46"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="54"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="40"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
       <c r="D50" s="43"/>
       <c r="E50" s="43"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="46"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="20"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="54"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="40"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
       <c r="D51" s="43"/>
       <c r="E51" s="43"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="46"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="20"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="54"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="40"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40"/>
       <c r="D52" s="43"/>
       <c r="E52" s="43"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="46"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="20"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="54"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="40"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="43"/>
       <c r="E53" s="43"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="46"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="54"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="40"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
       <c r="D54" s="43"/>
       <c r="E54" s="43"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="46"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="20"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="54"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="40"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
       <c r="D55" s="43"/>
       <c r="E55" s="43"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="46"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="20"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="54"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="40"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
       <c r="D56" s="43"/>
       <c r="E56" s="43"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="46"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="20"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="54"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="40"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
       <c r="D57" s="43"/>
       <c r="E57" s="43"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="46"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="20"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="54"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="40"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
       <c r="D58" s="43"/>
       <c r="E58" s="43"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="46"/>
-    </row>
-    <row r="59" spans="1:7" ht="128.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="21"/>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="54"/>
+    </row>
+    <row r="59" spans="1:8" ht="128.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="41"/>
+      <c r="B59" s="41"/>
+      <c r="C59" s="41"/>
       <c r="D59" s="44"/>
       <c r="E59" s="44"/>
-      <c r="F59" s="21"/>
-      <c r="G59" s="47"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="13" t="s">
+      <c r="F59" s="41"/>
+      <c r="G59" s="38"/>
+      <c r="H59" s="55"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C60" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="D60" s="39" t="s">
+      <c r="D60" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="E60" s="39" t="s">
+      <c r="E60" s="47" t="s">
         <v>161</v>
       </c>
-      <c r="F60" s="16" t="s">
+      <c r="F60" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="G60" s="45" t="s">
+      <c r="G60" s="36" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="14"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="40"/>
-      <c r="E61" s="40"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="46"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="14"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="40"/>
-      <c r="E62" s="40"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="46"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="40"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="46"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="14"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="40"/>
-      <c r="E64" s="40"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="46"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="14"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="40"/>
-      <c r="E65" s="40"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="46"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="14"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="40"/>
-      <c r="E66" s="40"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="46"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="14"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="40"/>
-      <c r="E67" s="40"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="46"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="14"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="40"/>
-      <c r="E68" s="40"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="46"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="14"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="40"/>
-      <c r="E69" s="40"/>
-      <c r="F69" s="17"/>
-      <c r="G69" s="46"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="14"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="40"/>
-      <c r="E70" s="40"/>
-      <c r="F70" s="17"/>
-      <c r="G70" s="46"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="14"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="40"/>
-      <c r="E71" s="40"/>
-      <c r="F71" s="17"/>
-      <c r="G71" s="46"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="14"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="40"/>
-      <c r="E72" s="40"/>
-      <c r="F72" s="17"/>
-      <c r="G72" s="46"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="14"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="40"/>
-      <c r="E73" s="40"/>
-      <c r="F73" s="17"/>
-      <c r="G73" s="46"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="14"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="40"/>
-      <c r="E74" s="40"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="46"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="14"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="40"/>
-      <c r="E75" s="40"/>
-      <c r="F75" s="17"/>
-      <c r="G75" s="46"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="14"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="40"/>
-      <c r="E76" s="40"/>
-      <c r="F76" s="17"/>
-      <c r="G76" s="46"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="14"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="40"/>
-      <c r="E77" s="40"/>
-      <c r="F77" s="17"/>
-      <c r="G77" s="46"/>
-    </row>
-    <row r="78" spans="1:7" ht="178.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="15"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="41"/>
-      <c r="E78" s="41"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="47"/>
+      <c r="H60" s="53" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="31"/>
+      <c r="B61" s="31"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="45"/>
+      <c r="E61" s="45"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="54"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="31"/>
+      <c r="B62" s="31"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="34"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="54"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="31"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="45"/>
+      <c r="E63" s="45"/>
+      <c r="F63" s="34"/>
+      <c r="G63" s="37"/>
+      <c r="H63" s="54"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="31"/>
+      <c r="B64" s="31"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="45"/>
+      <c r="E64" s="45"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="54"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="31"/>
+      <c r="B65" s="31"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
+      <c r="F65" s="34"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="54"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="31"/>
+      <c r="B66" s="31"/>
+      <c r="C66" s="31"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="45"/>
+      <c r="F66" s="34"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="54"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" s="31"/>
+      <c r="B67" s="31"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="45"/>
+      <c r="E67" s="45"/>
+      <c r="F67" s="34"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="54"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" s="31"/>
+      <c r="B68" s="31"/>
+      <c r="C68" s="31"/>
+      <c r="D68" s="45"/>
+      <c r="E68" s="45"/>
+      <c r="F68" s="34"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="54"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" s="31"/>
+      <c r="B69" s="31"/>
+      <c r="C69" s="31"/>
+      <c r="D69" s="45"/>
+      <c r="E69" s="45"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="37"/>
+      <c r="H69" s="54"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="31"/>
+      <c r="B70" s="31"/>
+      <c r="C70" s="31"/>
+      <c r="D70" s="45"/>
+      <c r="E70" s="45"/>
+      <c r="F70" s="34"/>
+      <c r="G70" s="37"/>
+      <c r="H70" s="54"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="31"/>
+      <c r="B71" s="31"/>
+      <c r="C71" s="31"/>
+      <c r="D71" s="45"/>
+      <c r="E71" s="45"/>
+      <c r="F71" s="34"/>
+      <c r="G71" s="37"/>
+      <c r="H71" s="54"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="31"/>
+      <c r="B72" s="31"/>
+      <c r="C72" s="31"/>
+      <c r="D72" s="45"/>
+      <c r="E72" s="45"/>
+      <c r="F72" s="34"/>
+      <c r="G72" s="37"/>
+      <c r="H72" s="54"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" s="31"/>
+      <c r="B73" s="31"/>
+      <c r="C73" s="31"/>
+      <c r="D73" s="45"/>
+      <c r="E73" s="45"/>
+      <c r="F73" s="34"/>
+      <c r="G73" s="37"/>
+      <c r="H73" s="54"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" s="31"/>
+      <c r="B74" s="31"/>
+      <c r="C74" s="31"/>
+      <c r="D74" s="45"/>
+      <c r="E74" s="45"/>
+      <c r="F74" s="34"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="54"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" s="31"/>
+      <c r="B75" s="31"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="45"/>
+      <c r="E75" s="45"/>
+      <c r="F75" s="34"/>
+      <c r="G75" s="37"/>
+      <c r="H75" s="54"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" s="31"/>
+      <c r="B76" s="31"/>
+      <c r="C76" s="31"/>
+      <c r="D76" s="45"/>
+      <c r="E76" s="45"/>
+      <c r="F76" s="34"/>
+      <c r="G76" s="37"/>
+      <c r="H76" s="54"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" s="31"/>
+      <c r="B77" s="31"/>
+      <c r="C77" s="31"/>
+      <c r="D77" s="45"/>
+      <c r="E77" s="45"/>
+      <c r="F77" s="34"/>
+      <c r="G77" s="37"/>
+      <c r="H77" s="54"/>
+    </row>
+    <row r="78" spans="1:8" ht="178.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="32"/>
+      <c r="B78" s="32"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="46"/>
+      <c r="E78" s="46"/>
+      <c r="F78" s="35"/>
+      <c r="G78" s="38"/>
+      <c r="H78" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="A13:A29"/>
-    <mergeCell ref="A30:A40"/>
-    <mergeCell ref="A41:A59"/>
-    <mergeCell ref="A60:A78"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="B13:B29"/>
-    <mergeCell ref="B30:B40"/>
-    <mergeCell ref="B41:B59"/>
-    <mergeCell ref="B60:B78"/>
+  <mergeCells count="40">
+    <mergeCell ref="H2:H12"/>
+    <mergeCell ref="H13:H29"/>
+    <mergeCell ref="H30:H40"/>
+    <mergeCell ref="H41:H59"/>
+    <mergeCell ref="H60:H78"/>
+    <mergeCell ref="C60:C78"/>
+    <mergeCell ref="F60:F78"/>
+    <mergeCell ref="G60:G78"/>
+    <mergeCell ref="D60:D78"/>
+    <mergeCell ref="E60:E78"/>
+    <mergeCell ref="C30:C40"/>
+    <mergeCell ref="F30:F40"/>
+    <mergeCell ref="G30:G40"/>
+    <mergeCell ref="C41:C59"/>
+    <mergeCell ref="F41:F59"/>
+    <mergeCell ref="G41:G59"/>
+    <mergeCell ref="D41:D59"/>
+    <mergeCell ref="D30:D40"/>
+    <mergeCell ref="E30:E40"/>
+    <mergeCell ref="E41:E59"/>
     <mergeCell ref="C2:C12"/>
     <mergeCell ref="F2:F12"/>
     <mergeCell ref="G2:G12"/>
@@ -4614,21 +4822,16 @@
     <mergeCell ref="D3:D12"/>
     <mergeCell ref="E2:E12"/>
     <mergeCell ref="E13:E29"/>
-    <mergeCell ref="C30:C40"/>
-    <mergeCell ref="F30:F40"/>
-    <mergeCell ref="G30:G40"/>
-    <mergeCell ref="C41:C59"/>
-    <mergeCell ref="F41:F59"/>
-    <mergeCell ref="G41:G59"/>
-    <mergeCell ref="D41:D59"/>
-    <mergeCell ref="D30:D40"/>
-    <mergeCell ref="E30:E40"/>
-    <mergeCell ref="E41:E59"/>
-    <mergeCell ref="C60:C78"/>
-    <mergeCell ref="F60:F78"/>
-    <mergeCell ref="G60:G78"/>
-    <mergeCell ref="D60:D78"/>
-    <mergeCell ref="E60:E78"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="B13:B29"/>
+    <mergeCell ref="B30:B40"/>
+    <mergeCell ref="B41:B59"/>
+    <mergeCell ref="B60:B78"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="A13:A29"/>
+    <mergeCell ref="A30:A40"/>
+    <mergeCell ref="A41:A59"/>
+    <mergeCell ref="A60:A78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>